<commit_message>
2 more test cases added to forgot password scenario
</commit_message>
<xml_diff>
--- a/bin/com/NFHS/xls/Forgot Password.xlsx
+++ b/bin/com/NFHS/xls/Forgot Password.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2490" windowWidth="13395" windowHeight="4215"/>
+    <workbookView xWindow="0" yWindow="2490" windowWidth="13395" windowHeight="4215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Forgot_Password3" sheetId="3" r:id="rId2"/>
+    <sheet name="Forgot_Password4" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D3"/>
+  <oleSize ref="A1:I12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>TCID</t>
   </si>
@@ -226,14 +227,29 @@
     <t>Forgot_Password15</t>
   </si>
   <si>
-    <t>Forgot_Password16</t>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>user1@gmail</t>
+  </si>
+  <si>
+    <t>user1@yopmail</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>user5@gmail.com</t>
+  </si>
+  <si>
+    <t>Forgot_Password4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +265,21 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -274,14 +305,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -294,8 +325,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="1"/>
@@ -599,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,253 +653,310 @@
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Forgot Password Scenario Completed
</commit_message>
<xml_diff>
--- a/bin/com/NFHS/xls/Forgot Password.xlsx
+++ b/bin/com/NFHS/xls/Forgot Password.xlsx
@@ -4,20 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2490" windowWidth="13395" windowHeight="4215" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18075" windowHeight="4110" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
     <sheet name="Forgot_Password3" sheetId="3" r:id="rId2"/>
     <sheet name="Forgot_Password4" sheetId="4" r:id="rId3"/>
+    <sheet name="Forgot_Password5" sheetId="5" r:id="rId4"/>
+    <sheet name="Forgot_Password7" sheetId="6" r:id="rId5"/>
+    <sheet name="Forgot_Password8" sheetId="7" r:id="rId6"/>
+    <sheet name="Forgot_Password9" sheetId="8" r:id="rId7"/>
+    <sheet name="Forgot_Password10" sheetId="9" r:id="rId8"/>
+    <sheet name="Forgot_Password11" sheetId="10" r:id="rId9"/>
+    <sheet name="Forgot_Password13" sheetId="11" r:id="rId10"/>
+    <sheet name="Forgot_Password14" sheetId="12" r:id="rId11"/>
+    <sheet name="Forgot_Password15" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:I12"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="62">
   <si>
     <t>TCID</t>
   </si>
@@ -244,12 +252,33 @@
   <si>
     <t>Forgot_Password4</t>
   </si>
+  <si>
+    <t>email@weboapps.com</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>weboqa6186</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>test1234</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +310,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -311,7 +346,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -334,6 +369,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -640,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,32 +746,32 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" s="13" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="D4" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="13" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>8</v>
+      <c r="D5" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -739,27 +784,36 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="D7" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="13" customFormat="1" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="12" t="s">
         <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -772,6 +826,9 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -783,6 +840,9 @@
       <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -794,6 +854,9 @@
       <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -805,16 +868,22 @@
       <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="10" t="s">
         <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="127.5" x14ac:dyDescent="0.25">
@@ -827,6 +896,9 @@
       <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -838,6 +910,9 @@
       <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -849,6 +924,9 @@
       <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
@@ -857,6 +935,187 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -919,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,4 +1218,360 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="email@weboapps.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
My Courses Distribution Scenario for Available Courses Completed
</commit_message>
<xml_diff>
--- a/bin/com/NFHS/xls/Forgot Password.xlsx
+++ b/bin/com/NFHS/xls/Forgot Password.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18075" windowHeight="4110" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="2490" windowWidth="17850" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -20,12 +20,13 @@
     <sheet name="Forgot_Password14" sheetId="12" r:id="rId11"/>
     <sheet name="Forgot_Password15" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A13:E14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>TCID</t>
   </si>
@@ -272,6 +273,12 @@
   </si>
   <si>
     <t>test123</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -685,17 +692,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,7 +736,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -743,7 +750,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="13" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
@@ -756,8 +763,8 @@
       <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>52</v>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="13" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -770,8 +777,8 @@
       <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>52</v>
+      <c r="D5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -785,7 +792,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="9" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -813,7 +820,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -827,7 +834,7 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
@@ -841,7 +848,7 @@
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.25">
@@ -855,7 +862,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="89.25" x14ac:dyDescent="0.25">
@@ -869,7 +876,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
@@ -882,7 +889,7 @@
       <c r="C13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -897,7 +904,7 @@
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
@@ -911,7 +918,7 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="114.75" x14ac:dyDescent="0.25">
@@ -926,6 +933,9 @@
       </c>
       <c r="D16" t="s">
         <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -948,11 +958,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1013,11 +1023,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1072,15 +1082,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1109,6 +1119,9 @@
       </c>
       <c r="C2" t="s">
         <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1129,10 +1142,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1184,10 +1197,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1230,9 +1243,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="2" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1282,9 +1295,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="4" width="25.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1345,10 +1358,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1397,10 +1410,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1455,11 +1468,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1520,12 +1533,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>